<commit_message>
Updated a lot: * Added 6_Documentation (editable Docs) * Changed Path to original Robot from TinkerCAD (link to their files) * Edited the PartLists and added all mechanical Components * Added an example video for Motion Tracking and for easier understanding what the code makes incl the corresponding hallsensor logs * Found a minor bug in the motionTracking and eddited the csv-Save
</commit_message>
<xml_diff>
--- a/1_HallSensor/11_Hardware/PartList.xlsx
+++ b/1_HallSensor/11_Hardware/PartList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_Local_Projekte\_PaperGitHub\MiniBumblebee_LowFieldMapping\1_HallSensor\11_Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83ED07E-CA0E-47D7-9AB3-E93BBF914490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC77F849-3A52-429D-BDA0-A1BDB4456F84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="6150" xr2:uid="{7BDEA584-2899-4DC0-97E4-FBE664656B29}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
   <si>
     <t>Order list for electronic components</t>
   </si>
@@ -286,6 +286,47 @@
   </si>
   <si>
     <t>could be any cheaper option</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>File Location</t>
+  </si>
+  <si>
+    <t>Mechanical Parts (Self Print etc)</t>
+  </si>
+  <si>
+    <t>How to manifacture</t>
+  </si>
+  <si>
+    <t>112_CAD Files\Base</t>
+  </si>
+  <si>
+    <t>* 3D Print or 
+* Laser Cutting or 
+* manual (sawing/drilling)</t>
+  </si>
+  <si>
+    <t>Base_Protection</t>
+  </si>
+  <si>
+    <t>112_CAD Files\SensorHead</t>
+  </si>
+  <si>
+    <t>* 3D Print (PETG)</t>
+  </si>
+  <si>
+    <t>Hallsensor_DistanceBolt_8mm4</t>
+  </si>
+  <si>
+    <t>Small Parts</t>
+  </si>
+  <si>
+    <t>M3 15mm Plastic Screws with washer/nut</t>
+  </si>
+  <si>
+    <t>Cable tie 2.5mm</t>
   </si>
 </sst>
 </file>
@@ -769,7 +810,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -780,6 +821,17 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1136,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D80811-2352-4897-A6C8-F4DC162DE13E}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1207,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1457,7 +1509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1477,7 +1529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1498,7 +1550,7 @@
       </c>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1518,7 +1570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1539,7 +1591,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -1562,12 +1614,102 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A4:G22">
     <sortCondition ref="B4:B22"/>

</xml_diff>